<commit_message>
Round 3 Input files
</commit_message>
<xml_diff>
--- a/BAOdev/OntoRatInputFiles/assay_cell_line_dev.xlsx
+++ b/BAOdev/OntoRatInputFiles/assay_cell_line_dev.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="79">
   <si>
     <t>Term ID</t>
   </si>
@@ -49,12 +49,6 @@
   </si>
   <si>
     <t>BJeLR</t>
-  </si>
-  <si>
-    <t>assay cell line</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/CLO_0000031</t>
   </si>
   <si>
     <t>BJeLR=BJ derivative also transformed with HRASV12; BJ fibroblasts were derived from primary human cells by transformation with hTERT, genomic SV40 Large T (LT) and Ssmall T (ST)</t>
@@ -190,6 +184,89 @@
   <si>
     <t>http://www.ncbi.nlm.nih.gov/books/NBK158949/?report=reader
 Patent (source of full descr): http://www.google.com/patents/WO2013192301A1?cl=en</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/CLO_0000019</t>
+  </si>
+  <si>
+    <t>immortal cell line cell</t>
+  </si>
+  <si>
+    <t>697 cell</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/CLO_0001008</t>
+  </si>
+  <si>
+    <t>Calu-1 cell</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/CLO_0002191</t>
+  </si>
+  <si>
+    <t>CHL-1 cell</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/CLO_0002420</t>
+  </si>
+  <si>
+    <t>DPX2 cell</t>
+  </si>
+  <si>
+    <t>DPX2 (aka DPX-2) is a HepG2-derived cell line stably integrated with a PXR (pregnane X receptor) expression vector plus a luciferase reporter, used to detect PXR activation/ CYP3A induction</t>
+  </si>
+  <si>
+    <t>http://www.ncbi.nlm.nih.gov/pubmed/15548381
+http://www.ncbi.nlm.nih.gov/pubmed/22912432</t>
+  </si>
+  <si>
+    <t>FA2N-4 cell</t>
+  </si>
+  <si>
+    <t>FA2N-4 is a human hepatocyte cell line; http://web.expasy.org/cellosaurus/CVCL_0267</t>
+  </si>
+  <si>
+    <t>http://purl.bioontology.org/ontology/MCCL/MCC_0000158
+http://cellfinder.org/ontology?id=CF_194407
+http://web.expasy.org/cellosaurus/CVCL_0267</t>
+  </si>
+  <si>
+    <t>HMC-1-8</t>
+  </si>
+  <si>
+    <t>HMC-1-8 is a human breast cancer cell line</t>
+  </si>
+  <si>
+    <t>http://web.expasy.org/cellosaurus/CVCL_2949
+http://portals.broadinstitute.org/ccle/cell%20lines/HMC18_BREAST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HMLE_sh_ECAD </t>
+  </si>
+  <si>
+    <t>HMLE_sh_ECAD is a stable cell line mimicking a cancer stem cell (CSC), derived by knocking down E-Cadherin (via shRNA) in human breast epithelial cells to induce epithelial to mesenchymal transition (EMT)</t>
+  </si>
+  <si>
+    <t>http://www.ncbi.nlm.nih.gov/pubmed/22941295
+http://www.ncbi.nlm.nih.gov/pubmed/19682730</t>
+  </si>
+  <si>
+    <t>HMLE_sh_eGFP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HMLE_sh_eGFP is a human breast epithelial cell line containing shRNA to GFP (green fluorescent reporter); used as an isogenic control line for HMLE_sh_ECAD </t>
+  </si>
+  <si>
+    <t>HMLE_sh_TWIST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HMLE_sh_TWIST is a stable cell line mimicking a cancer stem cell (CSC), derived by knocking down TWIST (via shRNA) in human breast epithelial cells to induce epithelial to mesenchymal transition (EMT); isogenic with another CSC line, HMLE_sh_ECAD </t>
+  </si>
+  <si>
+    <t>L6 cell</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/CLO_0007203</t>
   </si>
 </sst>
 </file>
@@ -198,12 +275,6 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <u/>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -223,6 +294,11 @@
       <sz val="12"/>
       <color rgb="FF222222"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF234979"/>
+      <name val="Lucida Sans Unicode"/>
     </font>
   </fonts>
   <fills count="5">
@@ -262,9 +338,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -280,13 +356,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -619,15 +700,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T16"/>
+  <dimension ref="A1:T26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="16384" width="11" style="1"/>
+    <col min="1" max="4" width="11" style="1"/>
+    <col min="5" max="5" width="59.83203125" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="63.75" customHeight="1">
@@ -678,363 +761,605 @@
         <v>2635</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="G2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="H2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" s="8">
+      <c r="I2" s="7">
         <v>42544</v>
       </c>
     </row>
     <row r="3" spans="1:20" ht="96" customHeight="1">
       <c r="B3" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C3" s="1">
         <v>493051</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="I3" s="8">
+      <c r="I3" s="7">
         <v>42544</v>
       </c>
     </row>
     <row r="4" spans="1:20" ht="31.5" customHeight="1">
-      <c r="B4" s="9" t="s">
-        <v>16</v>
+      <c r="B4" s="8" t="s">
+        <v>14</v>
       </c>
       <c r="C4" s="1">
         <v>743410</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>11</v>
+        <v>54</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="I4" s="8">
+        <v>16</v>
+      </c>
+      <c r="I4" s="7">
         <v>42513</v>
       </c>
     </row>
     <row r="5" spans="1:20" ht="31.5" customHeight="1">
       <c r="B5" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C5" s="1">
         <v>624379</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>11</v>
+        <v>54</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="I5" s="8">
+        <v>19</v>
+      </c>
+      <c r="I5" s="7">
         <v>42543</v>
       </c>
     </row>
     <row r="6" spans="1:20" ht="96" customHeight="1">
       <c r="B6" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C6" s="1">
         <v>2633</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="I6" s="8">
+      <c r="I6" s="7">
         <v>42544</v>
       </c>
     </row>
     <row r="7" spans="1:20" ht="240" customHeight="1">
       <c r="B7" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C7" s="1">
         <v>504574</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>11</v>
+        <v>54</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G7" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I7" s="7">
+        <v>42543</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" ht="63.75" customHeight="1">
+      <c r="B8" s="8" t="s">
         <v>25</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="I7" s="8">
-        <v>42543</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" ht="63.75" customHeight="1">
-      <c r="B8" s="9" t="s">
-        <v>27</v>
       </c>
       <c r="C8" s="1">
         <v>504341</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>11</v>
+        <v>54</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:20" ht="79.5" customHeight="1">
       <c r="B9" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C9" s="1">
         <v>504341</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>11</v>
+        <v>54</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="I9" s="8">
+        <v>30</v>
+      </c>
+      <c r="I9" s="7">
         <v>42543</v>
       </c>
     </row>
     <row r="10" spans="1:20" ht="127.5" customHeight="1">
       <c r="B10" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C10" s="1">
         <v>624467</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>11</v>
+        <v>54</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G10" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="I10" s="7">
+        <v>42545</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" ht="79.5" customHeight="1">
+      <c r="A11" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="H10" s="6" t="s">
+      <c r="B11" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="I10" s="8">
-        <v>42545</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" ht="79.5" customHeight="1">
-      <c r="A11" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>37</v>
       </c>
       <c r="C11" s="1">
         <v>488899</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>11</v>
+        <v>54</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="I11" s="8">
+        <v>37</v>
+      </c>
+      <c r="I11" s="7">
         <v>42535</v>
       </c>
     </row>
     <row r="12" spans="1:20" ht="79.5" customHeight="1">
       <c r="B12" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C12" s="1">
         <v>652144</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>11</v>
+        <v>54</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="I12" s="8">
+        <v>40</v>
+      </c>
+      <c r="I12" s="7">
         <v>42544</v>
       </c>
     </row>
     <row r="13" spans="1:20" ht="175.5" customHeight="1">
       <c r="B13" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C13" s="1">
         <v>588413</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G13" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="I13" s="7">
+        <v>42545</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" ht="15.75" customHeight="1">
+      <c r="A14" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="H13" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="I13" s="8">
-        <v>42545</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" ht="15.75" customHeight="1">
-      <c r="A14" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>46</v>
       </c>
       <c r="C14" s="1">
         <v>504653</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>11</v>
+        <v>54</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="I14" s="8">
+        <v>46</v>
+      </c>
+      <c r="I14" s="7">
         <v>42546</v>
       </c>
     </row>
     <row r="15" spans="1:20" ht="31.5" customHeight="1">
       <c r="B15" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C15" s="1">
         <v>463185</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>11</v>
+        <v>54</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H15" s="6"/>
-      <c r="I15" s="8">
+      <c r="I15" s="7">
         <v>42546</v>
       </c>
     </row>
     <row r="16" spans="1:20" ht="48" customHeight="1">
       <c r="B16" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C16" s="1">
         <v>651570</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>11</v>
+        <v>54</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="I16" s="8">
+        <v>51</v>
+      </c>
+      <c r="I16" s="7">
         <v>42545</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" ht="19">
+      <c r="B17" t="s">
+        <v>55</v>
+      </c>
+      <c r="C17">
+        <v>435022</v>
+      </c>
+      <c r="D17" t="s">
+        <v>54</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="F17"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="I17" s="13">
+        <v>42565</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9">
+      <c r="B18" t="s">
+        <v>57</v>
+      </c>
+      <c r="C18">
+        <v>602144</v>
+      </c>
+      <c r="D18" t="s">
+        <v>54</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="F18"/>
+      <c r="G18" s="12"/>
+      <c r="H18" t="s">
+        <v>58</v>
+      </c>
+      <c r="I18" s="13">
+        <v>42559</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" ht="19">
+      <c r="B19" t="s">
+        <v>59</v>
+      </c>
+      <c r="C19">
+        <v>504412</v>
+      </c>
+      <c r="D19" t="s">
+        <v>54</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="F19"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="I19" s="13">
+        <v>42557</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" ht="270">
+      <c r="B20" t="s">
+        <v>61</v>
+      </c>
+      <c r="C20">
+        <v>434939</v>
+      </c>
+      <c r="D20" t="s">
+        <v>54</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="F20"/>
+      <c r="G20" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="H20" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="I20" s="13">
+        <v>42552</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" ht="225">
+      <c r="B21" t="s">
+        <v>64</v>
+      </c>
+      <c r="C21">
+        <v>623928</v>
+      </c>
+      <c r="D21" t="s">
+        <v>54</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="F21"/>
+      <c r="G21" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="H21" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="I21" s="13">
+        <v>42557</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" ht="165">
+      <c r="B22" t="s">
+        <v>67</v>
+      </c>
+      <c r="C22">
+        <v>449755</v>
+      </c>
+      <c r="D22" t="s">
+        <v>54</v>
+      </c>
+      <c r="E22" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="F22"/>
+      <c r="G22" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="H22" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="I22" s="13">
+        <v>42554</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" ht="345">
+      <c r="B23" t="s">
+        <v>70</v>
+      </c>
+      <c r="C23">
+        <v>2717</v>
+      </c>
+      <c r="D23" t="s">
+        <v>54</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="F23"/>
+      <c r="G23" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="H23" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="I23" s="13">
+        <v>42569</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" ht="255">
+      <c r="B24" t="s">
+        <v>73</v>
+      </c>
+      <c r="C24">
+        <v>463074</v>
+      </c>
+      <c r="D24" t="s">
+        <v>54</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="F24"/>
+      <c r="G24" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="H24" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="I24" s="13">
+        <v>42569</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" ht="409">
+      <c r="B25" t="s">
+        <v>75</v>
+      </c>
+      <c r="C25">
+        <v>588703</v>
+      </c>
+      <c r="D25" t="s">
+        <v>54</v>
+      </c>
+      <c r="E25" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="F25"/>
+      <c r="G25" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="H25" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="I25" s="13">
+        <v>42569</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" ht="60">
+      <c r="B26" t="s">
+        <v>77</v>
+      </c>
+      <c r="C26">
+        <v>651895</v>
+      </c>
+      <c r="D26" t="s">
+        <v>54</v>
+      </c>
+      <c r="E26" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="F26"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="I26" s="13">
+        <v>42562</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E16" r:id="rId1"/>
-    <hyperlink ref="E15" r:id="rId2"/>
-    <hyperlink ref="E14" r:id="rId3"/>
-    <hyperlink ref="E13" r:id="rId4"/>
-    <hyperlink ref="E12" r:id="rId5"/>
-    <hyperlink ref="E11" r:id="rId6"/>
-    <hyperlink ref="E10" r:id="rId7"/>
-    <hyperlink ref="E9" r:id="rId8"/>
+    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="A11" r:id="rId2"/>
+    <hyperlink ref="A14" r:id="rId3"/>
+    <hyperlink ref="E3" r:id="rId4"/>
+    <hyperlink ref="E4" r:id="rId5"/>
+    <hyperlink ref="E5" r:id="rId6"/>
+    <hyperlink ref="E6" r:id="rId7"/>
+    <hyperlink ref="E7" r:id="rId8"/>
     <hyperlink ref="E8" r:id="rId9"/>
-    <hyperlink ref="E7" r:id="rId10"/>
-    <hyperlink ref="E6" r:id="rId11"/>
-    <hyperlink ref="E5" r:id="rId12"/>
-    <hyperlink ref="E4" r:id="rId13"/>
-    <hyperlink ref="E3" r:id="rId14"/>
-    <hyperlink ref="E2" r:id="rId15"/>
-    <hyperlink ref="A11" r:id="rId16"/>
-    <hyperlink ref="A14" r:id="rId17"/>
+    <hyperlink ref="E9" r:id="rId10"/>
+    <hyperlink ref="E10" r:id="rId11"/>
+    <hyperlink ref="E11" r:id="rId12"/>
+    <hyperlink ref="E12" r:id="rId13"/>
+    <hyperlink ref="E13" r:id="rId14"/>
+    <hyperlink ref="E14" r:id="rId15"/>
+    <hyperlink ref="E15" r:id="rId16"/>
+    <hyperlink ref="E16" r:id="rId17"/>
+    <hyperlink ref="E17" r:id="rId18"/>
+    <hyperlink ref="E18" r:id="rId19"/>
+    <hyperlink ref="E19" r:id="rId20"/>
+    <hyperlink ref="E20" r:id="rId21"/>
+    <hyperlink ref="E21" r:id="rId22"/>
+    <hyperlink ref="E22" r:id="rId23"/>
+    <hyperlink ref="E23" r:id="rId24"/>
+    <hyperlink ref="E24" r:id="rId25"/>
+    <hyperlink ref="E25" r:id="rId26"/>
+    <hyperlink ref="E26" r:id="rId27"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>